<commit_message>
Add Paper 5: Learning Multi-Attention Convolutional Neural Network for Fine-Grained Image Recognition
</commit_message>
<xml_diff>
--- a/Checkpoints & Updates/Checkpoints.xlsx
+++ b/Checkpoints & Updates/Checkpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meghp\Desktop\Ahmedabad University\Term 1\CSE618 Artificial Intelligence Laboratory\Bird Species Detection\Checkpoints &amp; Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FAD0D8-FC8B-40FE-8C43-1709D6379611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9D002C-0C97-4664-829A-5F98157D63B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1108,7 +1108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1149,6 +1149,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1156,15 +1159,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1474,15 +1468,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="37.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -1563,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896031BA-4B8A-4917-8DE1-F149FAC13D27}">
   <dimension ref="A1:F202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1595,39 +1589,39 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="17">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="11">
         <v>1</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="11">
         <f>E2</f>
         <v>60</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="12">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="17">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="11">
         <f>D2+1</f>
         <v>61</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="11">
         <f>E3+C3-1</f>
         <v>120</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="12">
         <v>60</v>
       </c>
     </row>
@@ -5439,407 +5433,407 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="19"/>
+    <col min="1" max="1" width="8.88671875" style="14"/>
     <col min="2" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="14" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="14" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="14" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="14" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="14" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="14" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="14" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="14" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="14" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="14" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="14" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="14" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="14" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="14" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="14" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="14" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="14" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="14" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="14" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="14" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="14" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="14" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="14" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="14" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="14" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="14" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="14" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="14" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="14" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="14" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="14" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="14" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="14" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="14" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="14" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="14" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="14" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="14" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="14" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="14" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="14" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="14" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="14" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="14" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="14" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="14" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="14" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="14" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="14" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="14" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="14" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="14" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="19" t="s">
+      <c r="A54" s="14" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="14" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="14" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="14" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="14" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="14" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="14" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="14" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="14" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="19" t="s">
+      <c r="A63" s="14" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="19" t="s">
+      <c r="A64" s="14" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="19" t="s">
+      <c r="A65" s="14" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="14" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="14" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="14" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="14" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="19" t="s">
+      <c r="A70" s="14" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="19" t="s">
+      <c r="A71" s="14" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="14" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="19" t="s">
+      <c r="A73" s="14" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="19" t="s">
+      <c r="A74" s="14" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="19" t="s">
+      <c r="A75" s="14" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="19" t="s">
+      <c r="A76" s="14" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="14" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="19" t="s">
+      <c r="A78" s="14" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="14" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="19" t="s">
+      <c r="A80" s="14" t="s">
         <v>301</v>
       </c>
     </row>

</xml_diff>